<commit_message>
Edited example files (added 'Сб' and 'Вс')
</commit_message>
<xml_diff>
--- a/data/example/01_01_2000.xlsx
+++ b/data/example/01_01_2000.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skrip\PythonApps\TimetableManager\data\example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skrip\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8B7599F5-E947-40D1-868C-CA444C374DD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46152350-0D49-4A0A-93CD-C5119D6CCCB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CBA0AA15-6431-431D-AAC9-9074CD7DCD66}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="45">
   <si>
     <t>День</t>
   </si>
@@ -173,6 +173,12 @@
   <si>
     <t>Пример Иванов И.И. 7
 Пример Иванова А.А. 17</t>
+  </si>
+  <si>
+    <t>Сб</t>
+  </si>
+  <si>
+    <t>Вс</t>
   </si>
 </sst>
 </file>
@@ -217,7 +223,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -242,33 +248,9 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
       <top style="thin">
         <color auto="1"/>
       </top>
@@ -308,19 +290,6 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
       <top style="thin">
         <color auto="1"/>
       </top>
@@ -402,10 +371,10 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -416,53 +385,70 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
@@ -471,38 +457,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -838,10 +796,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FAA225D-04B6-42D1-8AFD-4B55506516EB}">
-  <dimension ref="A1:F61"/>
+  <dimension ref="A1:F85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -866,822 +824,1068 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <v>1</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="6"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="4">
+      <c r="A3" s="18"/>
+      <c r="B3" s="3">
         <v>2</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="6"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="4">
+      <c r="A4" s="18"/>
+      <c r="B4" s="3">
         <v>3</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="6"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="4">
+      <c r="A5" s="18"/>
+      <c r="B5" s="3">
         <v>4</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="9"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="4">
+      <c r="A6" s="18"/>
+      <c r="B6" s="3">
         <v>5</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="9"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="4">
+      <c r="A7" s="18"/>
+      <c r="B7" s="3">
         <v>6</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="6"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="4">
+      <c r="A8" s="18"/>
+      <c r="B8" s="3">
         <v>7</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="5" t="s">
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="4">
+      <c r="A9" s="18"/>
+      <c r="B9" s="3">
         <v>8</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8" t="s">
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="4">
+      <c r="A10" s="18"/>
+      <c r="B10" s="3">
         <v>9</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5" t="s">
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="4">
+      <c r="A11" s="18"/>
+      <c r="B11" s="3">
         <v>10</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5" t="s">
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="4">
+      <c r="A12" s="18"/>
+      <c r="B12" s="3">
         <v>11</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5" t="s">
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="10"/>
-      <c r="B13" s="11">
+      <c r="A13" s="19"/>
+      <c r="B13" s="5">
         <v>12</v>
       </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="13"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
     </row>
     <row r="14" spans="1:6" ht="30.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="3">
         <v>1</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="9"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="4">
+      <c r="A15" s="18"/>
+      <c r="B15" s="3">
         <v>2</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="9"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="4"/>
     </row>
     <row r="16" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
-      <c r="B16" s="4">
+      <c r="A16" s="18"/>
+      <c r="B16" s="3">
         <v>3</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="5"/>
-      <c r="F16" s="9"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-      <c r="B17" s="4">
+      <c r="A17" s="18"/>
+      <c r="B17" s="3">
         <v>4</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="9"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="4"/>
     </row>
     <row r="18" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
-      <c r="B18" s="4">
+      <c r="A18" s="18"/>
+      <c r="B18" s="3">
         <v>5</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E18" s="5"/>
-      <c r="F18" s="9"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="4"/>
     </row>
     <row r="19" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="B19" s="4">
+      <c r="A19" s="18"/>
+      <c r="B19" s="3">
         <v>6</v>
       </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="9"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="B20" s="4">
+      <c r="A20" s="18"/>
+      <c r="B20" s="3">
         <v>7</v>
       </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="8" t="s">
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="F20" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="4">
+      <c r="A21" s="18"/>
+      <c r="B21" s="3">
         <v>8</v>
       </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5" t="s">
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F21" s="8" t="s">
+      <c r="F21" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
-      <c r="B22" s="4">
+      <c r="A22" s="18"/>
+      <c r="B22" s="3">
         <v>9</v>
       </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5" t="s">
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="F22" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
-      <c r="B23" s="4">
+      <c r="A23" s="18"/>
+      <c r="B23" s="3">
         <v>10</v>
       </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5" t="s">
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="F23" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" s="4">
+      <c r="A24" s="18"/>
+      <c r="B24" s="3">
         <v>11</v>
       </c>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5" t="s">
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="F24" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="10"/>
-      <c r="B25" s="11">
+      <c r="A25" s="19"/>
+      <c r="B25" s="5">
         <v>12</v>
       </c>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="13"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
     </row>
     <row r="26" spans="1:6" ht="30.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="14" t="s">
+      <c r="A26" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="15">
+      <c r="B26" s="8">
         <v>1</v>
       </c>
-      <c r="C26" s="16" t="s">
+      <c r="C26" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D26" s="16" t="s">
+      <c r="D26" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E26" s="17"/>
-      <c r="F26" s="18"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="9"/>
     </row>
     <row r="27" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
-      <c r="B27" s="15">
+      <c r="A27" s="18"/>
+      <c r="B27" s="8">
         <v>2</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="C27" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D27" s="16" t="s">
+      <c r="D27" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E27" s="17"/>
-      <c r="F27" s="18"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="9"/>
     </row>
     <row r="28" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
-      <c r="B28" s="15">
+      <c r="A28" s="18"/>
+      <c r="B28" s="8">
         <v>3</v>
       </c>
-      <c r="C28" s="16" t="s">
+      <c r="C28" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D28" s="16" t="s">
+      <c r="D28" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E28" s="17"/>
-      <c r="F28" s="19"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
     </row>
     <row r="29" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
-      <c r="B29" s="15">
+      <c r="A29" s="18"/>
+      <c r="B29" s="8">
         <v>4</v>
       </c>
-      <c r="C29" s="16" t="s">
+      <c r="C29" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D29" s="16" t="s">
+      <c r="D29" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E29" s="17"/>
-      <c r="F29" s="19"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
     </row>
     <row r="30" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
-      <c r="B30" s="15">
+      <c r="A30" s="18"/>
+      <c r="B30" s="8">
         <v>5</v>
       </c>
-      <c r="C30" s="16" t="s">
+      <c r="C30" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D30" s="16" t="s">
+      <c r="D30" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E30" s="17"/>
-      <c r="F30" s="19"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
     </row>
     <row r="31" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
-      <c r="B31" s="15">
+      <c r="A31" s="18"/>
+      <c r="B31" s="8">
         <v>6</v>
       </c>
-      <c r="C31" s="16" t="s">
+      <c r="C31" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D31" s="17"/>
-      <c r="E31" s="17" t="s">
+      <c r="D31" s="7"/>
+      <c r="E31" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F31" s="19"/>
+      <c r="F31" s="7"/>
     </row>
     <row r="32" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
-      <c r="B32" s="15">
+      <c r="A32" s="18"/>
+      <c r="B32" s="8">
         <v>7</v>
       </c>
-      <c r="C32" s="16" t="s">
+      <c r="C32" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D32" s="17"/>
-      <c r="E32" s="17" t="s">
+      <c r="D32" s="7"/>
+      <c r="E32" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F32" s="19"/>
+      <c r="F32" s="7"/>
     </row>
     <row r="33" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="7"/>
-      <c r="B33" s="15">
+      <c r="A33" s="18"/>
+      <c r="B33" s="8">
         <v>8</v>
       </c>
-      <c r="C33" s="17"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="17" t="s">
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F33" s="19" t="s">
+      <c r="F33" s="7" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="7"/>
-      <c r="B34" s="15">
+      <c r="A34" s="18"/>
+      <c r="B34" s="8">
         <v>9</v>
       </c>
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17" t="s">
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F34" s="19" t="s">
+      <c r="F34" s="7" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="7"/>
-      <c r="B35" s="15">
+      <c r="A35" s="18"/>
+      <c r="B35" s="8">
         <v>10</v>
       </c>
-      <c r="C35" s="17"/>
-      <c r="D35" s="17"/>
-      <c r="E35" s="17"/>
-      <c r="F35" s="19" t="s">
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="7"/>
-      <c r="B36" s="15">
+      <c r="A36" s="18"/>
+      <c r="B36" s="8">
         <v>11</v>
       </c>
-      <c r="C36" s="17"/>
-      <c r="D36" s="17"/>
-      <c r="E36" s="17"/>
-      <c r="F36" s="19" t="s">
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="10"/>
-      <c r="B37" s="20">
+      <c r="A37" s="19"/>
+      <c r="B37" s="10">
         <v>12</v>
       </c>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="21"/>
-      <c r="F37" s="22"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
     </row>
     <row r="38" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="23" t="s">
+      <c r="A38" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="B38" s="24">
+      <c r="B38" s="12">
         <v>1</v>
       </c>
-      <c r="C38" s="16" t="s">
+      <c r="C38" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D38" s="16" t="s">
+      <c r="D38" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E38" s="17"/>
-      <c r="F38" s="18"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="9"/>
     </row>
     <row r="39" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="25"/>
-      <c r="B39" s="15">
+      <c r="A39" s="22"/>
+      <c r="B39" s="8">
         <v>2</v>
       </c>
-      <c r="C39" s="16" t="s">
+      <c r="C39" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D39" s="16" t="s">
+      <c r="D39" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E39" s="17"/>
-      <c r="F39" s="18"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="9"/>
     </row>
     <row r="40" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="25"/>
-      <c r="B40" s="15">
+      <c r="A40" s="22"/>
+      <c r="B40" s="8">
         <v>3</v>
       </c>
-      <c r="C40" s="16" t="s">
+      <c r="C40" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D40" s="16" t="s">
+      <c r="D40" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E40" s="17"/>
-      <c r="F40" s="19"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
     </row>
     <row r="41" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="25"/>
-      <c r="B41" s="15">
+      <c r="A41" s="22"/>
+      <c r="B41" s="8">
         <v>4</v>
       </c>
-      <c r="C41" s="16" t="s">
+      <c r="C41" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D41" s="16" t="s">
+      <c r="D41" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E41" s="17"/>
-      <c r="F41" s="19"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
     </row>
     <row r="42" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="25"/>
-      <c r="B42" s="15">
+      <c r="A42" s="22"/>
+      <c r="B42" s="8">
         <v>5</v>
       </c>
-      <c r="C42" s="16" t="s">
+      <c r="C42" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D42" s="16" t="s">
+      <c r="D42" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E42" s="17"/>
-      <c r="F42" s="19"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
     </row>
     <row r="43" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="25"/>
-      <c r="B43" s="15">
+      <c r="A43" s="22"/>
+      <c r="B43" s="8">
         <v>6</v>
       </c>
-      <c r="C43" s="16" t="s">
+      <c r="C43" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D43" s="17"/>
-      <c r="E43" s="17" t="s">
+      <c r="D43" s="7"/>
+      <c r="E43" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F43" s="19"/>
+      <c r="F43" s="7"/>
     </row>
     <row r="44" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="25"/>
-      <c r="B44" s="15">
+      <c r="A44" s="22"/>
+      <c r="B44" s="8">
         <v>7</v>
       </c>
-      <c r="C44" s="16" t="s">
+      <c r="C44" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D44" s="17"/>
-      <c r="E44" s="17" t="s">
+      <c r="D44" s="7"/>
+      <c r="E44" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F44" s="19"/>
+      <c r="F44" s="7"/>
     </row>
     <row r="45" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="25"/>
-      <c r="B45" s="15">
+      <c r="A45" s="22"/>
+      <c r="B45" s="8">
         <v>8</v>
       </c>
-      <c r="C45" s="17"/>
-      <c r="D45" s="17"/>
-      <c r="E45" s="17" t="s">
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F45" s="19" t="s">
+      <c r="F45" s="7" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="25"/>
-      <c r="B46" s="15">
+      <c r="A46" s="22"/>
+      <c r="B46" s="8">
         <v>9</v>
       </c>
-      <c r="C46" s="17"/>
-      <c r="D46" s="17"/>
-      <c r="E46" s="17" t="s">
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F46" s="19" t="s">
+      <c r="F46" s="7" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="25"/>
-      <c r="B47" s="15">
+      <c r="A47" s="22"/>
+      <c r="B47" s="8">
         <v>10</v>
       </c>
-      <c r="C47" s="17"/>
-      <c r="D47" s="17"/>
-      <c r="E47" s="17"/>
-      <c r="F47" s="19" t="s">
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="25"/>
-      <c r="B48" s="15">
+      <c r="A48" s="22"/>
+      <c r="B48" s="8">
         <v>11</v>
       </c>
-      <c r="C48" s="17"/>
-      <c r="D48" s="17"/>
-      <c r="E48" s="17"/>
-      <c r="F48" s="19" t="s">
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="7" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="26"/>
-      <c r="B49" s="27">
+      <c r="A49" s="23"/>
+      <c r="B49" s="13">
         <v>12</v>
       </c>
-      <c r="C49" s="28"/>
-      <c r="D49" s="28"/>
-      <c r="E49" s="28"/>
-      <c r="F49" s="29"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
     </row>
     <row r="50" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="30" t="s">
+      <c r="A50" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="B50" s="31">
+      <c r="B50" s="16">
         <v>1</v>
       </c>
-      <c r="C50" s="16" t="s">
+      <c r="C50" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D50" s="16" t="s">
+      <c r="D50" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E50" s="17"/>
-      <c r="F50" s="18"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="9"/>
     </row>
     <row r="51" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="7"/>
-      <c r="B51" s="15">
+      <c r="A51" s="18"/>
+      <c r="B51" s="8">
         <v>2</v>
       </c>
-      <c r="C51" s="16" t="s">
+      <c r="C51" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D51" s="16" t="s">
+      <c r="D51" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E51" s="17"/>
-      <c r="F51" s="18"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="9"/>
     </row>
     <row r="52" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="7"/>
-      <c r="B52" s="15">
+      <c r="A52" s="18"/>
+      <c r="B52" s="8">
         <v>3</v>
       </c>
-      <c r="C52" s="16" t="s">
+      <c r="C52" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D52" s="16" t="s">
+      <c r="D52" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E52" s="17"/>
-      <c r="F52" s="19"/>
+      <c r="E52" s="7"/>
+      <c r="F52" s="7"/>
     </row>
     <row r="53" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="7"/>
-      <c r="B53" s="15">
+      <c r="A53" s="18"/>
+      <c r="B53" s="8">
         <v>4</v>
       </c>
-      <c r="C53" s="16" t="s">
+      <c r="C53" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D53" s="16" t="s">
+      <c r="D53" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E53" s="17"/>
-      <c r="F53" s="19"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="7"/>
     </row>
     <row r="54" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="7"/>
-      <c r="B54" s="15">
+      <c r="A54" s="18"/>
+      <c r="B54" s="8">
         <v>5</v>
       </c>
-      <c r="C54" s="16" t="s">
+      <c r="C54" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D54" s="16" t="s">
+      <c r="D54" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E54" s="17"/>
-      <c r="F54" s="19"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="7"/>
     </row>
     <row r="55" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="7"/>
-      <c r="B55" s="15">
+      <c r="A55" s="18"/>
+      <c r="B55" s="8">
         <v>6</v>
       </c>
-      <c r="C55" s="16" t="s">
+      <c r="C55" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="D55" s="17"/>
-      <c r="E55" s="17" t="s">
+      <c r="D55" s="7"/>
+      <c r="E55" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F55" s="19"/>
+      <c r="F55" s="7"/>
     </row>
     <row r="56" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="7"/>
-      <c r="B56" s="15">
+      <c r="A56" s="18"/>
+      <c r="B56" s="8">
         <v>7</v>
       </c>
-      <c r="C56" s="16" t="s">
+      <c r="C56" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D56" s="17"/>
-      <c r="E56" s="17" t="s">
+      <c r="D56" s="7"/>
+      <c r="E56" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F56" s="19"/>
+      <c r="F56" s="7"/>
     </row>
     <row r="57" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="7"/>
-      <c r="B57" s="15">
+      <c r="A57" s="18"/>
+      <c r="B57" s="8">
         <v>8</v>
       </c>
-      <c r="C57" s="17"/>
-      <c r="D57" s="17"/>
-      <c r="E57" s="17" t="s">
+      <c r="C57" s="7"/>
+      <c r="D57" s="7"/>
+      <c r="E57" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F57" s="19" t="s">
+      <c r="F57" s="7" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="7"/>
-      <c r="B58" s="15">
+      <c r="A58" s="18"/>
+      <c r="B58" s="8">
         <v>9</v>
       </c>
-      <c r="C58" s="17"/>
-      <c r="D58" s="17"/>
-      <c r="E58" s="17" t="s">
+      <c r="C58" s="7"/>
+      <c r="D58" s="7"/>
+      <c r="E58" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F58" s="19" t="s">
+      <c r="F58" s="7" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="7"/>
-      <c r="B59" s="15">
+      <c r="A59" s="18"/>
+      <c r="B59" s="8">
         <v>10</v>
       </c>
-      <c r="C59" s="17"/>
-      <c r="D59" s="17"/>
-      <c r="E59" s="17"/>
-      <c r="F59" s="19" t="s">
+      <c r="C59" s="7"/>
+      <c r="D59" s="7"/>
+      <c r="E59" s="7"/>
+      <c r="F59" s="7" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="7"/>
-      <c r="B60" s="15">
+      <c r="A60" s="18"/>
+      <c r="B60" s="8">
         <v>11</v>
       </c>
-      <c r="C60" s="17"/>
-      <c r="D60" s="17"/>
-      <c r="E60" s="17"/>
-      <c r="F60" s="19" t="s">
+      <c r="C60" s="7"/>
+      <c r="D60" s="7"/>
+      <c r="E60" s="7"/>
+      <c r="F60" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="7"/>
-      <c r="B61" s="20">
+    <row r="61" spans="1:6" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="18"/>
+      <c r="B61" s="13">
         <v>12</v>
       </c>
-      <c r="C61" s="21"/>
-      <c r="D61" s="21"/>
-      <c r="E61" s="21"/>
-      <c r="F61" s="22"/>
+      <c r="C61" s="14"/>
+      <c r="D61" s="14"/>
+      <c r="E61" s="14"/>
+      <c r="F61" s="14"/>
+    </row>
+    <row r="62" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B62" s="16">
+        <v>1</v>
+      </c>
+      <c r="C62" s="25"/>
+      <c r="D62" s="25"/>
+      <c r="E62" s="26"/>
+      <c r="F62" s="25"/>
+    </row>
+    <row r="63" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="18"/>
+      <c r="B63" s="8">
+        <v>2</v>
+      </c>
+      <c r="C63" s="9"/>
+      <c r="D63" s="9"/>
+      <c r="E63" s="7"/>
+      <c r="F63" s="9"/>
+    </row>
+    <row r="64" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="18"/>
+      <c r="B64" s="8">
+        <v>3</v>
+      </c>
+      <c r="C64" s="9"/>
+      <c r="D64" s="9"/>
+      <c r="E64" s="7"/>
+      <c r="F64" s="7"/>
+    </row>
+    <row r="65" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="18"/>
+      <c r="B65" s="8">
+        <v>4</v>
+      </c>
+      <c r="C65" s="9"/>
+      <c r="D65" s="9"/>
+      <c r="E65" s="7"/>
+      <c r="F65" s="7"/>
+    </row>
+    <row r="66" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="18"/>
+      <c r="B66" s="8">
+        <v>5</v>
+      </c>
+      <c r="C66" s="9"/>
+      <c r="D66" s="9"/>
+      <c r="E66" s="7"/>
+      <c r="F66" s="7"/>
+    </row>
+    <row r="67" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="18"/>
+      <c r="B67" s="8">
+        <v>6</v>
+      </c>
+      <c r="C67" s="9"/>
+      <c r="D67" s="7"/>
+      <c r="E67" s="7"/>
+      <c r="F67" s="7"/>
+    </row>
+    <row r="68" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="18"/>
+      <c r="B68" s="8">
+        <v>7</v>
+      </c>
+      <c r="C68" s="9"/>
+      <c r="D68" s="7"/>
+      <c r="E68" s="7"/>
+      <c r="F68" s="7"/>
+    </row>
+    <row r="69" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="18"/>
+      <c r="B69" s="8">
+        <v>8</v>
+      </c>
+      <c r="C69" s="7"/>
+      <c r="D69" s="7"/>
+      <c r="E69" s="7"/>
+      <c r="F69" s="7"/>
+    </row>
+    <row r="70" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="18"/>
+      <c r="B70" s="8">
+        <v>9</v>
+      </c>
+      <c r="C70" s="7"/>
+      <c r="D70" s="7"/>
+      <c r="E70" s="7"/>
+      <c r="F70" s="7"/>
+    </row>
+    <row r="71" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="18"/>
+      <c r="B71" s="8">
+        <v>10</v>
+      </c>
+      <c r="C71" s="7"/>
+      <c r="D71" s="7"/>
+      <c r="E71" s="7"/>
+      <c r="F71" s="7"/>
+    </row>
+    <row r="72" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="18"/>
+      <c r="B72" s="8">
+        <v>11</v>
+      </c>
+      <c r="C72" s="7"/>
+      <c r="D72" s="7"/>
+      <c r="E72" s="7"/>
+      <c r="F72" s="7"/>
+    </row>
+    <row r="73" spans="1:6" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="18"/>
+      <c r="B73" s="13">
+        <v>12</v>
+      </c>
+      <c r="C73" s="14"/>
+      <c r="D73" s="14"/>
+      <c r="E73" s="14"/>
+      <c r="F73" s="14"/>
+    </row>
+    <row r="74" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="B74" s="12">
+        <v>1</v>
+      </c>
+      <c r="C74" s="27"/>
+      <c r="D74" s="27"/>
+      <c r="E74" s="15"/>
+      <c r="F74" s="27"/>
+    </row>
+    <row r="75" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="18"/>
+      <c r="B75" s="8">
+        <v>2</v>
+      </c>
+      <c r="C75" s="9"/>
+      <c r="D75" s="9"/>
+      <c r="E75" s="7"/>
+      <c r="F75" s="9"/>
+    </row>
+    <row r="76" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="18"/>
+      <c r="B76" s="8">
+        <v>3</v>
+      </c>
+      <c r="C76" s="9"/>
+      <c r="D76" s="9"/>
+      <c r="E76" s="7"/>
+      <c r="F76" s="7"/>
+    </row>
+    <row r="77" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="18"/>
+      <c r="B77" s="8">
+        <v>4</v>
+      </c>
+      <c r="C77" s="9"/>
+      <c r="D77" s="9"/>
+      <c r="E77" s="7"/>
+      <c r="F77" s="7"/>
+    </row>
+    <row r="78" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="18"/>
+      <c r="B78" s="8">
+        <v>5</v>
+      </c>
+      <c r="C78" s="9"/>
+      <c r="D78" s="9"/>
+      <c r="E78" s="7"/>
+      <c r="F78" s="7"/>
+    </row>
+    <row r="79" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="18"/>
+      <c r="B79" s="8">
+        <v>6</v>
+      </c>
+      <c r="C79" s="9"/>
+      <c r="D79" s="7"/>
+      <c r="E79" s="7"/>
+      <c r="F79" s="7"/>
+    </row>
+    <row r="80" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="18"/>
+      <c r="B80" s="8">
+        <v>7</v>
+      </c>
+      <c r="C80" s="9"/>
+      <c r="D80" s="7"/>
+      <c r="E80" s="7"/>
+      <c r="F80" s="7"/>
+    </row>
+    <row r="81" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="18"/>
+      <c r="B81" s="8">
+        <v>8</v>
+      </c>
+      <c r="C81" s="7"/>
+      <c r="D81" s="7"/>
+      <c r="E81" s="7"/>
+      <c r="F81" s="7"/>
+    </row>
+    <row r="82" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="18"/>
+      <c r="B82" s="8">
+        <v>9</v>
+      </c>
+      <c r="C82" s="7"/>
+      <c r="D82" s="7"/>
+      <c r="E82" s="7"/>
+      <c r="F82" s="7"/>
+    </row>
+    <row r="83" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="18"/>
+      <c r="B83" s="8">
+        <v>10</v>
+      </c>
+      <c r="C83" s="7"/>
+      <c r="D83" s="7"/>
+      <c r="E83" s="7"/>
+      <c r="F83" s="7"/>
+    </row>
+    <row r="84" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="18"/>
+      <c r="B84" s="8">
+        <v>11</v>
+      </c>
+      <c r="C84" s="7"/>
+      <c r="D84" s="7"/>
+      <c r="E84" s="7"/>
+      <c r="F84" s="7"/>
+    </row>
+    <row r="85" spans="1:6" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="28"/>
+      <c r="B85" s="13">
+        <v>12</v>
+      </c>
+      <c r="C85" s="14"/>
+      <c r="D85" s="14"/>
+      <c r="E85" s="14"/>
+      <c r="F85" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
+    <mergeCell ref="A62:A73"/>
+    <mergeCell ref="A74:A85"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="A14:A25"/>
     <mergeCell ref="A26:A37"/>

</xml_diff>